<commit_message>
added reference number to forest plots in main manuscript
added excel file with all references and associated numbers
added function in utils.R to add reference number to correct study in datAll
amended script to run this
all results updated
</commit_message>
<xml_diff>
--- a/results/serotonin_studies.xlsx
+++ b/results/serotonin_studies.xlsx
@@ -1,545 +1,538 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/11679a5894e85aa0/POSTDOC/PROJECT_MetaAnalysis/DA5HT_MetaAnalysis_public/results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_E98293383C996BE7A8B52C39073817D13AD86802" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{639DC9F9-05D6-C64C-8C84-B660A775AD28}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="171">
-  <si>
-    <t>Study</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Drug, Dose</t>
-  </si>
-  <si>
-    <t>N drug</t>
-  </si>
-  <si>
-    <t>N placebo</t>
-  </si>
-  <si>
-    <t>Original design</t>
-  </si>
-  <si>
-    <t>Final design</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Outcome</t>
-  </si>
-  <si>
-    <t>Study Age</t>
-  </si>
-  <si>
-    <t>Study Female Proportion</t>
-  </si>
-  <si>
-    <t>Drug regimen</t>
-  </si>
-  <si>
-    <t>Colwell, 2024</t>
-  </si>
-  <si>
-    <t>R L/S</t>
-  </si>
-  <si>
-    <t>fenfluramine 15mg b.i.d.</t>
-  </si>
-  <si>
-    <t>bw</t>
-  </si>
-  <si>
-    <t>PILT</t>
-  </si>
-  <si>
-    <t>learning rate</t>
-  </si>
-  <si>
-    <t>20.17</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>&gt;1</t>
-  </si>
-  <si>
-    <t>Cools, 2008</t>
-  </si>
-  <si>
-    <t>TD</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>observational reversal</t>
-  </si>
-  <si>
-    <t>non-reversal errors</t>
-  </si>
-  <si>
-    <t>22.4</t>
-  </si>
-  <si>
-    <t>0.67</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Finger, 2007</t>
-  </si>
-  <si>
-    <t>PAL</t>
-  </si>
-  <si>
-    <t>omission errors</t>
-  </si>
-  <si>
-    <t>27.94</t>
-  </si>
-  <si>
-    <t>0.52</t>
-  </si>
-  <si>
-    <t>Gilger, 2024</t>
-  </si>
-  <si>
-    <t>w†</t>
-  </si>
-  <si>
-    <t>Two-step</t>
-  </si>
-  <si>
-    <t>main effect reward</t>
-  </si>
-  <si>
-    <t>32.2</t>
-  </si>
-  <si>
-    <t>0.38</t>
-  </si>
-  <si>
-    <t>Jepma, 2010</t>
-  </si>
-  <si>
-    <t>citalopram 30mg</t>
-  </si>
-  <si>
-    <t>restless bandit</t>
-  </si>
-  <si>
-    <t>inverse temperature</t>
-  </si>
-  <si>
-    <t>21.55</t>
-  </si>
-  <si>
-    <t>0.49</t>
-  </si>
-  <si>
-    <t>Luo, 2024</t>
-  </si>
-  <si>
-    <t>escitalopram 20mg</t>
-  </si>
-  <si>
-    <t>probabilistic reversal</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Michely, 2022</t>
-  </si>
-  <si>
-    <t>citalopram 20mg/day</t>
-  </si>
-  <si>
-    <t>gambling card</t>
-  </si>
-  <si>
-    <t>24.65</t>
-  </si>
-  <si>
-    <t>0.39</t>
-  </si>
-  <si>
-    <t>Robinson, 2012</t>
-  </si>
-  <si>
-    <t>27.6</t>
-  </si>
-  <si>
-    <t>Seymour, 2012</t>
-  </si>
-  <si>
-    <t>sensitivity</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>R S</t>
-  </si>
-  <si>
-    <t>outcome sensitivity</t>
-  </si>
-  <si>
-    <t>P L/S</t>
-  </si>
-  <si>
-    <t>P S</t>
-  </si>
-  <si>
-    <t>Geurts, 2013</t>
-  </si>
-  <si>
-    <t>P+</t>
-  </si>
-  <si>
-    <t>PIT</t>
-  </si>
-  <si>
-    <t>appetitive PIT</t>
-  </si>
-  <si>
-    <t>23.8</t>
-  </si>
-  <si>
-    <t>Guitart-Masip, 2012</t>
-  </si>
-  <si>
-    <t>citalopram 24mg oral</t>
-  </si>
-  <si>
-    <t>go/nogo</t>
-  </si>
-  <si>
-    <t>nogo to win</t>
-  </si>
-  <si>
-    <t>23.3</t>
-  </si>
-  <si>
-    <t>Guitart-Masip, 2014</t>
-  </si>
-  <si>
-    <t>Hebart, 2015</t>
-  </si>
-  <si>
-    <t>appetative PIT</t>
-  </si>
-  <si>
-    <t>P-</t>
-  </si>
-  <si>
-    <t>Crockett, 2009</t>
-  </si>
-  <si>
-    <t>go/nogo RT</t>
-  </si>
-  <si>
-    <t>punishment-induced slowing</t>
-  </si>
-  <si>
-    <t>Crockett, 2012</t>
-  </si>
-  <si>
-    <t>Gaber, 2015</t>
-  </si>
-  <si>
-    <t>25.34</t>
-  </si>
-  <si>
-    <t>aversive PIT</t>
-  </si>
-  <si>
-    <t>go to avoid</t>
-  </si>
-  <si>
-    <t>Helmbold, 2015</t>
-  </si>
-  <si>
-    <t>24.22</t>
-  </si>
-  <si>
-    <t>Crean, 2002</t>
-  </si>
-  <si>
-    <t>RD</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>k parameter</t>
-  </si>
-  <si>
-    <t>21.5</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Schweighofer, 2008</t>
-  </si>
-  <si>
-    <t>DD dynamic</t>
-  </si>
-  <si>
-    <t>discount factor gamma</t>
-  </si>
-  <si>
-    <t>Tanaka, 2007</t>
-  </si>
-  <si>
-    <t>multi-step DD</t>
-  </si>
-  <si>
-    <t>p(large reward choices)</t>
-  </si>
-  <si>
-    <t>Worbe, 2014</t>
-  </si>
-  <si>
-    <t>28.97</t>
-  </si>
-  <si>
-    <t>0.61</t>
-  </si>
-  <si>
-    <t>Beierholm, 2013</t>
-  </si>
-  <si>
-    <t>RV</t>
-  </si>
-  <si>
-    <t>odd-ball discrimination</t>
-  </si>
-  <si>
-    <t>average reward rate on RTs</t>
-  </si>
-  <si>
-    <t>23.91</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>Cools, 2005</t>
-  </si>
-  <si>
-    <t>CRRT</t>
-  </si>
-  <si>
-    <t>RT 90-10</t>
-  </si>
-  <si>
-    <t>23.55</t>
-  </si>
-  <si>
-    <t>Roiser, 2006</t>
-  </si>
-  <si>
-    <t>26.75</t>
-  </si>
-  <si>
-    <t>0.43</t>
-  </si>
-  <si>
-    <t>Steding, 2023</t>
-  </si>
-  <si>
-    <t>physical effort</t>
-  </si>
-  <si>
-    <t>button press high-low</t>
-  </si>
-  <si>
-    <t>Chamberlain, 2006</t>
-  </si>
-  <si>
-    <t>MB/F</t>
-  </si>
-  <si>
-    <t>reversal</t>
-  </si>
-  <si>
-    <t>perseverative errors</t>
-  </si>
-  <si>
-    <t>25.82</t>
-  </si>
-  <si>
-    <t>switch errors</t>
-  </si>
-  <si>
-    <t>Evers, 2004</t>
-  </si>
-  <si>
-    <t>21.8</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>omega parameter</t>
-  </si>
-  <si>
-    <t>Kanen, 2020</t>
-  </si>
-  <si>
-    <t>perseveration</t>
-  </si>
-  <si>
-    <t>0.47</t>
-  </si>
-  <si>
-    <t>Langley, 2023</t>
-  </si>
-  <si>
-    <t>escitalopram 20mg /day</t>
-  </si>
-  <si>
-    <t>Two-step task</t>
-  </si>
-  <si>
-    <t>Reward × Transition</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>65.17</t>
-  </si>
-  <si>
-    <t>Skandali, 2018</t>
-  </si>
-  <si>
-    <t>Probabilistic reversal</t>
-  </si>
-  <si>
-    <t>reversal errors</t>
-  </si>
-  <si>
-    <t>Thirkettle, 2019</t>
-  </si>
-  <si>
-    <t>Tryptophan 0.8g</t>
-  </si>
-  <si>
-    <t>21.1</t>
-  </si>
-  <si>
-    <t>0.64</t>
-  </si>
-  <si>
-    <t>Worbe, 2015</t>
-  </si>
-  <si>
-    <t>3-stage instrumental learning</t>
-  </si>
-  <si>
-    <t>devalued choices</t>
-  </si>
-  <si>
-    <t>26.33</t>
-  </si>
-  <si>
-    <t>0.56</t>
-  </si>
-  <si>
-    <t>Worbe, 2016</t>
-  </si>
-  <si>
-    <t>29.14</t>
-  </si>
-  <si>
-    <t>Anderson, 2003</t>
-  </si>
-  <si>
-    <t>RA</t>
-  </si>
-  <si>
-    <t>gambling</t>
-  </si>
-  <si>
-    <t>mean indifference odds against win</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Campbell-Meiklejohn, 2011</t>
-  </si>
-  <si>
-    <t>p(gamble)</t>
-  </si>
-  <si>
-    <t>24.18</t>
-  </si>
-  <si>
-    <t>0.53</t>
-  </si>
-  <si>
-    <t>Faulkner, 2017</t>
-  </si>
-  <si>
-    <t>29.45</t>
-  </si>
-  <si>
-    <t>0.54</t>
-  </si>
-  <si>
-    <t>Macoveanu, 2014</t>
-  </si>
-  <si>
-    <t>fluoxetine 20/40mg/day</t>
-  </si>
-  <si>
-    <t>p(risky choice)</t>
-  </si>
-  <si>
-    <t>Murphy, 2009</t>
-  </si>
-  <si>
-    <t>l-tryptophan 3g/day</t>
-  </si>
-  <si>
-    <t>25.54</t>
-  </si>
-  <si>
-    <t>Rogers, 2003</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
+  <si>
+    <t xml:space="preserve">Study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug, Dose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N drug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N placebo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study Female Proportion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug regimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colwell, 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R L/S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fenfluramine 15mg b.i.d.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PILT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">learning rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cools, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">observational reversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-reversal errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finger, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omission errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gilger, 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w†</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two-step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main effect reward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jepma, 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">citalopram 30mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restless bandit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverse temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luo, 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escitalopram 20mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">probabilistic reversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michely, 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">citalopram 20mg/day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gambling card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robinson, 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seymour, 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outcome sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P L/S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geurts, 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appetitive PIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guitart-Masip, 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">citalopram 24mg oral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go/nogo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nogo to win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guitart-Masip, 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hebart, 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appetative PIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crockett, 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go/nogo RT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">punishment-induced slowing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crockett, 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaber, 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aversive PIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go to avoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helmbold, 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crean, 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweighofer, 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD dynamic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discount factor gamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanaka, 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multi-step DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p(large reward choices)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worbe, 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beierholm, 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">odd-ball discrimination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average reward rate on RTs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cools, 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT 90-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roiser, 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steding, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">physical effort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button press high-low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chamberlain, 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MB/F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perseverative errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evers, 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omega parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kanen, 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perseveration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Langley, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escitalopram 20mg /day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two-step task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reward × Transition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skandali, 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probabilistic reversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reversal errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thirkettle, 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tryptophan 0.8g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worbe, 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-stage instrumental learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">devalued choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worbe, 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anderson, 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gambling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean indifference odds against win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campbell-Meiklejohn, 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p(gamble)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faulkner, 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macoveanu, 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fluoxetine 20/40mg/day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p(risky choice)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murphy, 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l-tryptophan 3g/day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rogers, 2003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -575,15 +568,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -865,19 +849,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -915,7 +894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -925,10 +904,10 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>26</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>27</v>
       </c>
       <c r="F2" t="s">
@@ -953,7 +932,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -963,10 +942,10 @@
       <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>12</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>12</v>
       </c>
       <c r="F3" t="s">
@@ -991,7 +970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1001,10 +980,10 @@
       <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>19</v>
       </c>
       <c r="F4" t="s">
@@ -1029,7 +1008,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1039,10 +1018,10 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>98</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>98</v>
       </c>
       <c r="F5" t="s">
@@ -1067,7 +1046,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1077,10 +1056,10 @@
       <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>16</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>17</v>
       </c>
       <c r="F6" t="s">
@@ -1105,7 +1084,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1115,10 +1094,10 @@
       <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>32</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>33</v>
       </c>
       <c r="F7" t="s">
@@ -1143,7 +1122,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1153,10 +1132,10 @@
       <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>33</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>33</v>
       </c>
       <c r="F8" t="s">
@@ -1181,7 +1160,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1191,10 +1170,10 @@
       <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>21</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>20</v>
       </c>
       <c r="F9" t="s">
@@ -1219,7 +1198,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1229,10 +1208,10 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D10">
-        <v>15</v>
-      </c>
-      <c r="E10">
+      <c r="D10" t="n">
+        <v>15</v>
+      </c>
+      <c r="E10" t="n">
         <v>15</v>
       </c>
       <c r="F10" t="s">
@@ -1257,7 +1236,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1267,10 +1246,10 @@
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>26</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>27</v>
       </c>
       <c r="F11" t="s">
@@ -1295,7 +1274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1305,10 +1284,10 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>26</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>27</v>
       </c>
       <c r="F12" t="s">
@@ -1333,7 +1312,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1343,10 +1322,10 @@
       <c r="C13" t="s">
         <v>47</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>32</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>33</v>
       </c>
       <c r="F13" t="s">
@@ -1371,7 +1350,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1381,10 +1360,10 @@
       <c r="C14" t="s">
         <v>51</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>33</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>33</v>
       </c>
       <c r="F14" t="s">
@@ -1409,7 +1388,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -1419,10 +1398,10 @@
       <c r="C15" t="s">
         <v>22</v>
       </c>
-      <c r="D15">
-        <v>15</v>
-      </c>
-      <c r="E15">
+      <c r="D15" t="n">
+        <v>15</v>
+      </c>
+      <c r="E15" t="n">
         <v>15</v>
       </c>
       <c r="F15" t="s">
@@ -1447,7 +1426,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1457,10 +1436,10 @@
       <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>26</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>27</v>
       </c>
       <c r="F16" t="s">
@@ -1485,7 +1464,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1495,10 +1474,10 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="n">
         <v>45</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>45</v>
       </c>
       <c r="F17" t="s">
@@ -1523,7 +1502,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1533,10 +1512,10 @@
       <c r="C18" t="s">
         <v>70</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>16</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>20</v>
       </c>
       <c r="F18" t="s">
@@ -1561,7 +1540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -1571,10 +1550,10 @@
       <c r="C19" t="s">
         <v>41</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="n">
         <v>27</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>29</v>
       </c>
       <c r="F19" t="s">
@@ -1599,7 +1578,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -1609,10 +1588,10 @@
       <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="n">
         <v>34</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="n">
         <v>34</v>
       </c>
       <c r="F20" t="s">
@@ -1637,7 +1616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1647,10 +1626,10 @@
       <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="n">
         <v>12</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="n">
         <v>12</v>
       </c>
       <c r="F21" t="s">
@@ -1675,7 +1654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -1685,10 +1664,10 @@
       <c r="C22" t="s">
         <v>22</v>
       </c>
-      <c r="D22">
-        <v>22</v>
-      </c>
-      <c r="E22">
+      <c r="D22" t="n">
+        <v>22</v>
+      </c>
+      <c r="E22" t="n">
         <v>22</v>
       </c>
       <c r="F22" t="s">
@@ -1713,7 +1692,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1723,10 +1702,10 @@
       <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="n">
         <v>24</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="n">
         <v>24</v>
       </c>
       <c r="F23" t="s">
@@ -1751,7 +1730,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -1761,10 +1740,10 @@
       <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="n">
         <v>24</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="n">
         <v>24</v>
       </c>
       <c r="F24" t="s">
@@ -1789,7 +1768,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -1799,10 +1778,10 @@
       <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>45</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>45</v>
       </c>
       <c r="F25" t="s">
@@ -1827,7 +1806,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -1837,10 +1816,10 @@
       <c r="C26" t="s">
         <v>70</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>16</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>20</v>
       </c>
       <c r="F26" t="s">
@@ -1865,7 +1844,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -1875,10 +1854,10 @@
       <c r="C27" t="s">
         <v>41</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="n">
         <v>27</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>29</v>
       </c>
       <c r="F27" t="s">
@@ -1903,7 +1882,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -1913,10 +1892,10 @@
       <c r="C28" t="s">
         <v>22</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="n">
         <v>34</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="n">
         <v>34</v>
       </c>
       <c r="F28" t="s">
@@ -1941,7 +1920,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -1951,10 +1930,10 @@
       <c r="C29" t="s">
         <v>22</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="n">
         <v>18</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="n">
         <v>18</v>
       </c>
       <c r="F29" t="s">
@@ -1979,7 +1958,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1989,10 +1968,10 @@
       <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="n">
         <v>21</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="n">
         <v>20</v>
       </c>
       <c r="F30" t="s">
@@ -2017,7 +1996,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -2027,10 +2006,10 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>20</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>20</v>
       </c>
       <c r="F31" t="s">
@@ -2055,7 +2034,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2065,10 +2044,10 @@
       <c r="C32" t="s">
         <v>22</v>
       </c>
-      <c r="D32">
+      <c r="D32" t="n">
         <v>20</v>
       </c>
-      <c r="E32">
+      <c r="E32" t="n">
         <v>20</v>
       </c>
       <c r="F32" t="s">
@@ -2093,7 +2072,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -2103,10 +2082,10 @@
       <c r="C33" t="s">
         <v>22</v>
       </c>
-      <c r="D33">
+      <c r="D33" t="n">
         <v>12</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="n">
         <v>12</v>
       </c>
       <c r="F33" t="s">
@@ -2131,7 +2110,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -2141,10 +2120,10 @@
       <c r="C34" t="s">
         <v>22</v>
       </c>
-      <c r="D34">
-        <v>22</v>
-      </c>
-      <c r="E34">
+      <c r="D34" t="n">
+        <v>22</v>
+      </c>
+      <c r="E34" t="n">
         <v>22</v>
       </c>
       <c r="F34" t="s">
@@ -2169,7 +2148,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -2179,10 +2158,10 @@
       <c r="C35" t="s">
         <v>70</v>
       </c>
-      <c r="D35">
+      <c r="D35" t="n">
         <v>30</v>
       </c>
-      <c r="E35">
+      <c r="E35" t="n">
         <v>30</v>
       </c>
       <c r="F35" t="s">
@@ -2207,7 +2186,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -2217,10 +2196,10 @@
       <c r="C36" t="s">
         <v>22</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="n">
         <v>10</v>
       </c>
-      <c r="E36">
+      <c r="E36" t="n">
         <v>12</v>
       </c>
       <c r="F36" t="s">
@@ -2245,7 +2224,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" t="s">
         <v>113</v>
       </c>
@@ -2255,10 +2234,10 @@
       <c r="C37" t="s">
         <v>22</v>
       </c>
-      <c r="D37">
+      <c r="D37" t="n">
         <v>30</v>
       </c>
-      <c r="E37">
+      <c r="E37" t="n">
         <v>30</v>
       </c>
       <c r="F37" t="s">
@@ -2283,7 +2262,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" t="s">
         <v>116</v>
       </c>
@@ -2293,10 +2272,10 @@
       <c r="C38" t="s">
         <v>22</v>
       </c>
-      <c r="D38">
+      <c r="D38" t="n">
         <v>24</v>
       </c>
-      <c r="E38">
+      <c r="E38" t="n">
         <v>24</v>
       </c>
       <c r="F38" t="s">
@@ -2321,7 +2300,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -2331,10 +2310,10 @@
       <c r="C39" t="s">
         <v>41</v>
       </c>
-      <c r="D39">
+      <c r="D39" t="n">
         <v>20</v>
       </c>
-      <c r="E39">
+      <c r="E39" t="n">
         <v>20</v>
       </c>
       <c r="F39" t="s">
@@ -2359,7 +2338,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -2369,10 +2348,10 @@
       <c r="C40" t="s">
         <v>22</v>
       </c>
-      <c r="D40">
+      <c r="D40" t="n">
         <v>12</v>
       </c>
-      <c r="E40">
+      <c r="E40" t="n">
         <v>12</v>
       </c>
       <c r="F40" t="s">
@@ -2397,7 +2376,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" t="s">
         <v>125</v>
       </c>
@@ -2407,10 +2386,10 @@
       <c r="C41" t="s">
         <v>22</v>
       </c>
-      <c r="D41">
-        <v>15</v>
-      </c>
-      <c r="E41">
+      <c r="D41" t="n">
+        <v>15</v>
+      </c>
+      <c r="E41" t="n">
         <v>15</v>
       </c>
       <c r="F41" t="s">
@@ -2435,7 +2414,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" t="s">
         <v>34</v>
       </c>
@@ -2445,10 +2424,10 @@
       <c r="C42" t="s">
         <v>22</v>
       </c>
-      <c r="D42">
+      <c r="D42" t="n">
         <v>98</v>
       </c>
-      <c r="E42">
+      <c r="E42" t="n">
         <v>98</v>
       </c>
       <c r="F42" t="s">
@@ -2473,7 +2452,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" t="s">
         <v>129</v>
       </c>
@@ -2483,10 +2462,10 @@
       <c r="C43" t="s">
         <v>22</v>
       </c>
-      <c r="D43">
+      <c r="D43" t="n">
         <v>30</v>
       </c>
-      <c r="E43">
+      <c r="E43" t="n">
         <v>32</v>
       </c>
       <c r="F43" t="s">
@@ -2511,7 +2490,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" t="s">
         <v>132</v>
       </c>
@@ -2521,10 +2500,10 @@
       <c r="C44" t="s">
         <v>133</v>
       </c>
-      <c r="D44">
+      <c r="D44" t="n">
         <v>32</v>
       </c>
-      <c r="E44">
+      <c r="E44" t="n">
         <v>34</v>
       </c>
       <c r="F44" t="s">
@@ -2549,7 +2528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" t="s">
         <v>138</v>
       </c>
@@ -2559,10 +2538,10 @@
       <c r="C45" t="s">
         <v>47</v>
       </c>
-      <c r="D45">
+      <c r="D45" t="n">
         <v>31</v>
       </c>
-      <c r="E45">
+      <c r="E45" t="n">
         <v>33</v>
       </c>
       <c r="F45" t="s">
@@ -2587,7 +2566,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" t="s">
         <v>141</v>
       </c>
@@ -2597,10 +2576,10 @@
       <c r="C46" t="s">
         <v>142</v>
       </c>
-      <c r="D46">
-        <v>22</v>
-      </c>
-      <c r="E46">
+      <c r="D46" t="n">
+        <v>22</v>
+      </c>
+      <c r="E46" t="n">
         <v>22</v>
       </c>
       <c r="F46" t="s">
@@ -2625,7 +2604,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" t="s">
         <v>145</v>
       </c>
@@ -2635,10 +2614,10 @@
       <c r="C47" t="s">
         <v>22</v>
       </c>
-      <c r="D47">
+      <c r="D47" t="n">
         <v>18</v>
       </c>
-      <c r="E47">
+      <c r="E47" t="n">
         <v>18</v>
       </c>
       <c r="F47" t="s">
@@ -2663,7 +2642,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" t="s">
         <v>150</v>
       </c>
@@ -2673,10 +2652,10 @@
       <c r="C48" t="s">
         <v>22</v>
       </c>
-      <c r="D48">
-        <v>22</v>
-      </c>
-      <c r="E48">
+      <c r="D48" t="n">
+        <v>22</v>
+      </c>
+      <c r="E48" t="n">
         <v>22</v>
       </c>
       <c r="F48" t="s">
@@ -2701,7 +2680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" t="s">
         <v>152</v>
       </c>
@@ -2711,10 +2690,10 @@
       <c r="C49" t="s">
         <v>22</v>
       </c>
-      <c r="D49">
-        <v>15</v>
-      </c>
-      <c r="E49">
+      <c r="D49" t="n">
+        <v>15</v>
+      </c>
+      <c r="E49" t="n">
         <v>13</v>
       </c>
       <c r="F49" t="s">
@@ -2739,7 +2718,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" t="s">
         <v>157</v>
       </c>
@@ -2749,10 +2728,10 @@
       <c r="C50" t="s">
         <v>22</v>
       </c>
-      <c r="D50">
+      <c r="D50" t="n">
         <v>17</v>
       </c>
-      <c r="E50">
+      <c r="E50" t="n">
         <v>17</v>
       </c>
       <c r="F50" t="s">
@@ -2777,7 +2756,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" t="s">
         <v>161</v>
       </c>
@@ -2787,10 +2766,10 @@
       <c r="C51" t="s">
         <v>22</v>
       </c>
-      <c r="D51">
+      <c r="D51" t="n">
         <v>26</v>
       </c>
-      <c r="E51">
+      <c r="E51" t="n">
         <v>26</v>
       </c>
       <c r="F51" t="s">
@@ -2815,7 +2794,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" t="s">
         <v>164</v>
       </c>
@@ -2825,10 +2804,10 @@
       <c r="C52" t="s">
         <v>165</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="n">
         <v>13</v>
       </c>
-      <c r="E52">
+      <c r="E52" t="n">
         <v>16</v>
       </c>
       <c r="F52" t="s">
@@ -2853,7 +2832,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" t="s">
         <v>167</v>
       </c>
@@ -2863,10 +2842,10 @@
       <c r="C53" t="s">
         <v>168</v>
       </c>
-      <c r="D53">
-        <v>15</v>
-      </c>
-      <c r="E53">
+      <c r="D53" t="n">
+        <v>15</v>
+      </c>
+      <c r="E53" t="n">
         <v>15</v>
       </c>
       <c r="F53" t="s">
@@ -2891,7 +2870,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" t="s">
         <v>170</v>
       </c>
@@ -2901,10 +2880,10 @@
       <c r="C54" t="s">
         <v>22</v>
       </c>
-      <c r="D54">
+      <c r="D54" t="n">
         <v>18</v>
       </c>
-      <c r="E54">
+      <c r="E54" t="n">
         <v>18</v>
       </c>
       <c r="F54" t="s">
@@ -2931,6 +2910,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>